<commit_message>
updated preclass documentation with ooxml parse errors
</commit_message>
<xml_diff>
--- a/docs/ClamAV_Document_Properties.xlsx
+++ b/docs/ClamAV_Document_Properties.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="525" windowWidth="27495" windowHeight="10680"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Overview" state="visible" r:id="rId3"/>
-    <sheet sheetId="2" name="PE Sections" state="visible" r:id="rId4"/>
+    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="PE Sections" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="354">
   <si>
     <t>All Documents</t>
   </si>
@@ -620,8 +623,7 @@
     <t>Company(string)*</t>
   </si>
   <si>
-    <t>
-</t>
+    <t/>
   </si>
   <si>
     <t>SignedCount(int)</t>
@@ -1033,26 +1035,83 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_CORE_XMLPARSER</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_CORE_MALFORMED</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_EXTN_XMLPARSER</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_EXTN_MALFORMED</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_XML_READER_FD</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_MULTIPLE_CORE_PROPFILES</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_MISSING_CORE_PROPFILES</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_MULTIPLE_EXTN_PROPFILES</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_MISSING_EXTN_PROPFILES</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_MULTIPLE_CUSTOM_PROPFILES</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_MISSING_CUST_PROPFILES</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_TIMEOUT</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_NO_CONTENT_TYPES</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_OUTOFMEM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1060,7 +1119,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="none"/>
@@ -1079,1223 +1138,1657 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment/>
-    </xf>
-    <xf fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2"/>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
-      <alignment/>
-    </xf>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E34" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="35.0"/>
-    <col min="2" customWidth="1" max="2" width="31.57"/>
-    <col min="3" customWidth="1" max="3" width="24.43"/>
-    <col min="4" customWidth="1" max="6" width="45.57"/>
-    <col min="7" customWidth="1" max="9" width="38.0"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="6" width="45.5703125" customWidth="1"/>
+    <col min="7" max="9" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="1" r="E1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="1" r="F1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="G1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="1" r="H1">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="1" r="I1">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c s="2" r="J1"/>
-      <c s="2" r="K1"/>
-      <c s="2" r="L1"/>
-      <c s="2" r="M1"/>
-      <c s="2" r="N1"/>
-      <c s="2" r="O1"/>
-      <c s="2" r="P1"/>
-      <c s="2" r="Q1"/>
-      <c s="2" r="R1"/>
-      <c s="2" r="S1"/>
-      <c s="2" r="T1"/>
-      <c s="2" r="U1"/>
-      <c s="2" r="V1"/>
-      <c s="2" r="W1"/>
-      <c s="2" r="X1"/>
-      <c s="2" r="Y1"/>
-      <c s="2" r="Z1"/>
-    </row>
-    <row r="2">
-      <c t="s" s="3" r="A2">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="3" r="B2">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="3" r="C2">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="3" r="D2">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="3" r="E2">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="3" r="F2">
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="3" r="G2">
+      <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="3" r="H2">
+      <c r="H2" s="3" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="3" r="I2">
+      <c r="I2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="3" r="A3">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="3" r="B3">
+      <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="3" r="C3">
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="3" r="D3">
+      <c r="D3" s="3" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="3" r="E3">
+      <c r="E3" s="3" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="3" r="F3">
+      <c r="F3" s="3" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="3" r="G3">
+      <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="3" r="H3">
+      <c r="H3" s="3" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="3" r="I3">
+      <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" s="3" r="A4">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="3" r="B4">
+      <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="3" r="C4">
+      <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="3" r="D4">
+      <c r="D4" s="3" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="3" r="E4">
+      <c r="E4" s="3" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="3" r="F4">
+      <c r="F4" s="3" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="3" r="G4">
+      <c r="G4" s="3" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="3" r="H4">
+      <c r="H4" s="3" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="3" r="I4">
+      <c r="I4" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" s="3" r="A5">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="3" r="B5">
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="3" r="C5">
+      <c r="C5" s="3" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="3" r="D5">
+      <c r="D5" s="3" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="3" r="E5">
+      <c r="E5" s="3" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="3" r="F5">
+      <c r="F5" s="3" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="3" r="G5">
+      <c r="G5" s="3" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="3" r="H5">
+      <c r="H5" s="3" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="3" r="I5">
+      <c r="I5" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" s="3" r="A6">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="3" r="B6">
+      <c r="B6" s="3" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="3" r="C6">
+      <c r="C6" s="3" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="3" r="G6">
+      <c r="G6" s="3" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="3" r="H6">
+      <c r="H6" s="3" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="3" r="I6">
+      <c r="I6" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" s="3" r="A7">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="3" r="B7">
+      <c r="B7" s="3" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="3" r="C7">
+      <c r="C7" s="3" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="3" r="D7">
+      <c r="D7" s="3" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="3" r="E7">
+      <c r="E7" s="3" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="3" r="F7">
+      <c r="F7" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8">
-      <c t="s" s="3" r="B8">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="3" r="C8">
+      <c r="C8" s="3" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="3" r="D8">
+      <c r="D8" s="3" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="3" r="E8">
+      <c r="E8" s="3" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="3" r="F8">
+      <c r="F8" s="3" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="3" r="G8">
+      <c r="G8" s="3" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="3" r="H8">
+      <c r="H8" s="3" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="3" r="I8">
+      <c r="I8" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9">
-      <c t="s" s="3" r="B9">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
         <v>65</v>
       </c>
-      <c t="s" s="3" r="C9">
+      <c r="C9" s="3" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="3" r="D9">
+      <c r="D9" s="3" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="3" r="E9">
+      <c r="E9" s="3" t="s">
         <v>68</v>
       </c>
-      <c t="s" s="3" r="F9">
+      <c r="F9" s="3" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="3" r="G9">
+      <c r="G9" s="3" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="3" r="H9">
+      <c r="H9" s="3" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="3" r="I9">
+      <c r="I9" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10">
-      <c t="s" s="3" r="B10">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
         <v>73</v>
       </c>
-      <c t="s" s="3" r="C10">
+      <c r="C10" s="3" t="s">
         <v>74</v>
       </c>
-      <c t="s" s="3" r="D10">
+      <c r="D10" s="3" t="s">
         <v>75</v>
       </c>
-      <c t="s" s="3" r="E10">
+      <c r="E10" s="3" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="3" r="F10">
+      <c r="F10" s="3" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="3" r="G10">
+      <c r="G10" s="3" t="s">
         <v>78</v>
       </c>
-      <c t="s" s="3" r="H10">
+      <c r="H10" s="3" t="s">
         <v>79</v>
       </c>
-      <c t="s" s="3" r="I10">
+      <c r="I10" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" s="3" r="B11">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
         <v>81</v>
       </c>
-      <c t="s" s="3" r="C11">
+      <c r="C11" s="3" t="s">
         <v>82</v>
       </c>
-      <c t="s" s="3" r="D11">
+      <c r="D11" s="3" t="s">
         <v>83</v>
       </c>
-      <c t="s" s="3" r="E11">
+      <c r="E11" s="3" t="s">
         <v>84</v>
       </c>
-      <c t="s" s="3" r="F11">
+      <c r="F11" s="3" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="3" r="G11">
+      <c r="G11" s="3" t="s">
         <v>86</v>
       </c>
-      <c t="s" s="3" r="H11">
+      <c r="H11" s="3" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="3" r="I11">
+      <c r="I11" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12">
-      <c t="s" s="3" r="B12">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
         <v>89</v>
       </c>
-      <c t="s" s="3" r="C12">
+      <c r="C12" s="3" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="3" r="D12">
+      <c r="D12" s="3" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="3" r="E12">
+      <c r="E12" s="3" t="s">
         <v>92</v>
       </c>
-      <c t="s" s="3" r="F12">
+      <c r="F12" s="3" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="3" r="G12">
+      <c r="G12" s="3" t="s">
         <v>94</v>
       </c>
-      <c t="s" s="3" r="H12">
+      <c r="H12" s="3" t="s">
         <v>95</v>
       </c>
-      <c t="s" s="3" r="I12">
+      <c r="I12" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13">
-      <c t="s" s="3" r="B13">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="3" r="C13">
+      <c r="C13" s="3" t="s">
         <v>98</v>
       </c>
-      <c t="s" s="3" r="D13">
+      <c r="D13" s="3" t="s">
         <v>99</v>
       </c>
-      <c t="s" s="3" r="E13">
+      <c r="E13" s="3" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="3" r="F13">
+      <c r="F13" s="3" t="s">
         <v>101</v>
       </c>
-      <c t="s" s="3" r="G13">
+      <c r="G13" s="3" t="s">
         <v>102</v>
       </c>
-      <c t="s" s="3" r="H13">
+      <c r="H13" s="3" t="s">
         <v>103</v>
       </c>
-      <c t="s" s="3" r="I13">
+      <c r="I13" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14">
-      <c t="s" s="3" r="B14">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>105</v>
       </c>
-      <c t="s" s="3" r="C14">
+      <c r="C14" s="3" t="s">
         <v>106</v>
       </c>
-      <c t="s" s="3" r="D14">
+      <c r="D14" s="3" t="s">
         <v>107</v>
       </c>
-      <c t="s" s="3" r="E14">
+      <c r="E14" s="3" t="s">
         <v>108</v>
       </c>
-      <c t="s" s="3" r="F14">
+      <c r="F14" s="3" t="s">
         <v>109</v>
       </c>
-      <c t="s" s="3" r="G14">
+      <c r="G14" s="3" t="s">
         <v>110</v>
       </c>
-      <c t="s" s="3" r="H14">
+      <c r="H14" s="3" t="s">
         <v>111</v>
       </c>
-      <c t="s" s="3" r="I14">
+      <c r="I14" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15">
-      <c t="s" s="3" r="B15">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
         <v>113</v>
       </c>
-      <c t="s" s="3" r="C15">
+      <c r="C15" s="3" t="s">
         <v>114</v>
       </c>
-      <c t="s" s="3" r="D15">
+      <c r="D15" s="3" t="s">
         <v>115</v>
       </c>
-      <c t="s" s="3" r="E15">
+      <c r="E15" s="3" t="s">
         <v>116</v>
       </c>
-      <c t="s" s="3" r="F15">
+      <c r="F15" s="3" t="s">
         <v>117</v>
       </c>
-      <c t="s" s="3" r="G15">
+      <c r="G15" s="3" t="s">
         <v>118</v>
       </c>
-      <c t="s" s="3" r="H15">
+      <c r="H15" s="3" t="s">
         <v>119</v>
       </c>
-      <c t="s" s="3" r="I15">
+      <c r="I15" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="16">
-      <c t="s" s="3" r="B16">
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="3" r="C16">
+      <c r="C16" s="3" t="s">
         <v>122</v>
       </c>
-      <c t="s" s="3" r="D16">
+      <c r="D16" s="3" t="s">
         <v>123</v>
       </c>
-      <c t="s" s="3" r="E16">
+      <c r="E16" s="3" t="s">
         <v>124</v>
       </c>
-      <c t="s" s="3" r="F16">
+      <c r="F16" s="3" t="s">
         <v>125</v>
       </c>
-      <c t="s" s="3" r="G16">
+      <c r="G16" s="3" t="s">
         <v>126</v>
       </c>
-      <c t="s" s="3" r="H16">
+      <c r="H16" s="3" t="s">
         <v>127</v>
       </c>
-      <c t="s" s="3" r="I16">
+      <c r="I16" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="17">
-      <c t="s" s="3" r="B17">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
         <v>129</v>
       </c>
-      <c t="s" s="3" r="C17">
+      <c r="C17" s="3" t="s">
         <v>130</v>
       </c>
-      <c t="s" s="3" r="D17">
+      <c r="D17" s="3" t="s">
         <v>131</v>
       </c>
-      <c t="s" s="3" r="E17">
+      <c r="E17" s="3" t="s">
         <v>132</v>
       </c>
-      <c t="s" s="3" r="F17">
+      <c r="F17" s="3" t="s">
         <v>133</v>
       </c>
-      <c t="s" s="3" r="G17">
+      <c r="G17" s="3" t="s">
         <v>134</v>
       </c>
-      <c t="s" s="3" r="H17">
+      <c r="H17" s="3" t="s">
         <v>135</v>
       </c>
-      <c t="s" s="3" r="I17">
+      <c r="I17" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18">
-      <c t="s" s="3" r="B18">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
         <v>137</v>
       </c>
-      <c t="s" s="3" r="C18">
+      <c r="C18" s="3" t="s">
         <v>138</v>
       </c>
-      <c t="s" s="3" r="D18">
+      <c r="D18" s="3" t="s">
         <v>139</v>
       </c>
-      <c t="s" s="3" r="E18">
+      <c r="E18" s="3" t="s">
         <v>140</v>
       </c>
-      <c t="s" s="3" r="F18">
+      <c r="F18" s="3" t="s">
         <v>141</v>
       </c>
-      <c t="s" s="3" r="G18">
+      <c r="G18" s="3" t="s">
         <v>142</v>
       </c>
-      <c t="s" s="3" r="H18">
+      <c r="H18" s="3" t="s">
         <v>143</v>
       </c>
-      <c t="s" s="3" r="I18">
+      <c r="I18" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="19">
-      <c t="s" s="3" r="B19">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
         <v>145</v>
       </c>
-      <c t="s" s="3" r="C19">
+      <c r="C19" s="3" t="s">
         <v>146</v>
       </c>
-      <c t="s" s="3" r="D19">
+      <c r="D19" s="3" t="s">
         <v>147</v>
       </c>
-      <c t="s" s="3" r="E19">
+      <c r="E19" s="3" t="s">
         <v>148</v>
       </c>
-      <c t="s" s="3" r="F19">
+      <c r="F19" s="3" t="s">
         <v>149</v>
       </c>
-      <c t="s" s="3" r="G19">
+      <c r="G19" s="3" t="s">
         <v>150</v>
       </c>
-      <c t="s" s="3" r="H19">
+      <c r="H19" s="3" t="s">
         <v>151</v>
       </c>
-      <c t="s" s="3" r="I19">
+      <c r="I19" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="20">
-      <c t="s" s="3" r="B20">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
         <v>153</v>
       </c>
-      <c t="s" s="3" r="C20">
+      <c r="C20" s="3" t="s">
         <v>154</v>
       </c>
-      <c t="s" s="3" r="D20">
+      <c r="D20" s="3" t="s">
         <v>155</v>
       </c>
-      <c t="s" s="3" r="E20">
+      <c r="E20" s="3" t="s">
         <v>156</v>
       </c>
-      <c t="s" s="3" r="F20">
+      <c r="F20" s="3" t="s">
         <v>157</v>
       </c>
-      <c t="s" s="3" r="G20">
+      <c r="G20" s="3" t="s">
         <v>158</v>
       </c>
-      <c t="s" s="3" r="H20">
+      <c r="H20" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="21">
-      <c t="s" s="3" r="B21">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>160</v>
       </c>
-      <c t="s" s="3" r="C21">
+      <c r="C21" s="3" t="s">
         <v>161</v>
       </c>
-      <c t="s" s="3" r="D21">
+      <c r="D21" s="3" t="s">
         <v>162</v>
       </c>
-      <c t="s" s="3" r="E21">
+      <c r="E21" s="3" t="s">
         <v>163</v>
       </c>
-      <c t="s" s="3" r="I21">
+      <c r="I21" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22">
-      <c t="s" s="3" r="B22">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>165</v>
       </c>
-      <c t="s" s="3" r="C22">
+      <c r="C22" s="3" t="s">
         <v>166</v>
       </c>
-      <c t="s" s="3" r="D22">
+      <c r="D22" s="3" t="s">
         <v>167</v>
       </c>
-      <c t="s" s="3" r="F22">
+      <c r="F22" s="3" t="s">
         <v>168</v>
       </c>
-      <c t="s" s="3" r="G22">
+      <c r="G22" s="3" t="s">
         <v>169</v>
       </c>
-      <c t="s" s="3" r="H22">
+      <c r="H22" s="3" t="s">
         <v>170</v>
       </c>
-      <c t="s" s="3" r="I22">
+      <c r="I22" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="23">
-      <c t="s" s="3" r="B23">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>172</v>
       </c>
-      <c t="s" s="3" r="C23">
+      <c r="C23" s="3" t="s">
         <v>173</v>
       </c>
-      <c t="s" s="3" r="D23">
+      <c r="D23" s="3" t="s">
         <v>174</v>
       </c>
-      <c t="s" s="3" r="E23">
+      <c r="E23" s="3" t="s">
         <v>175</v>
       </c>
-      <c t="s" s="3" r="F23">
+      <c r="F23" s="3" t="s">
         <v>176</v>
       </c>
-      <c t="s" s="3" r="G23">
+      <c r="G23" s="3" t="s">
         <v>177</v>
       </c>
-      <c t="s" s="3" r="H23">
+      <c r="H23" s="3" t="s">
         <v>178</v>
       </c>
-      <c t="s" s="3" r="I23">
+      <c r="I23" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="24">
-      <c t="s" s="3" r="B24">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
         <v>180</v>
       </c>
-      <c t="s" s="3" r="C24">
+      <c r="C24" s="3" t="s">
         <v>181</v>
       </c>
-      <c t="s" s="3" r="D24">
+      <c r="D24" s="3" t="s">
         <v>182</v>
       </c>
-      <c t="s" s="3" r="E24">
+      <c r="E24" s="3" t="s">
         <v>183</v>
       </c>
-      <c t="s" s="3" r="F24">
+      <c r="F24" s="3" t="s">
         <v>184</v>
       </c>
-      <c t="s" s="3" r="G24">
+      <c r="G24" s="3" t="s">
         <v>185</v>
       </c>
-      <c t="s" s="3" r="H24">
+      <c r="H24" s="3" t="s">
         <v>186</v>
       </c>
-      <c t="s" s="3" r="I24">
+      <c r="I24" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="25">
-      <c t="s" s="3" r="B25">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>188</v>
       </c>
-      <c t="s" s="3" r="C25">
+      <c r="C25" s="3" t="s">
         <v>189</v>
       </c>
-      <c t="s" s="3" r="D25">
+      <c r="D25" s="3" t="s">
         <v>190</v>
       </c>
-      <c t="s" s="3" r="E25">
+      <c r="E25" s="3" t="s">
         <v>191</v>
       </c>
-      <c t="s" s="3" r="F25">
+      <c r="F25" s="3" t="s">
         <v>192</v>
       </c>
-      <c t="s" s="3" r="G25">
+      <c r="G25" s="3" t="s">
         <v>193</v>
       </c>
-      <c t="s" s="3" r="H25">
+      <c r="H25" s="3" t="s">
         <v>194</v>
       </c>
-      <c t="s" s="3" r="I25">
+      <c r="I25" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="26">
-      <c t="s" s="3" r="B26">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
         <v>196</v>
       </c>
-      <c t="s" s="3" r="E26">
+      <c r="E26" s="3" t="s">
         <v>197</v>
       </c>
-      <c t="s" s="3" r="F26">
+      <c r="F26" s="3" t="s">
         <v>198</v>
       </c>
-      <c t="s" s="3" r="G26">
+      <c r="G26" s="3" t="s">
         <v>199</v>
       </c>
-      <c t="s" s="3" r="H26">
+      <c r="H26" s="3" t="s">
         <v>200</v>
       </c>
-      <c t="s" s="3" r="I26">
+      <c r="I26" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="27">
-      <c t="s" s="3" r="A27">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>202</v>
       </c>
-      <c t="s" s="3" r="B27">
+      <c r="B27" s="3" t="s">
         <v>203</v>
       </c>
-      <c t="s" s="3" r="D27">
+      <c r="D27" s="3" t="s">
         <v>204</v>
       </c>
-      <c t="s" s="3" r="E27">
+      <c r="E27" s="3" t="s">
         <v>205</v>
       </c>
-      <c t="s" s="3" r="F27">
+      <c r="F27" s="3" t="s">
         <v>206</v>
       </c>
-      <c t="s" s="3" r="G27">
+      <c r="G27" s="3" t="s">
         <v>207</v>
       </c>
-      <c t="s" s="3" r="H27">
+      <c r="H27" s="3" t="s">
         <v>208</v>
       </c>
-      <c t="s" s="3" r="I27">
+      <c r="I27" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="28">
-      <c t="s" s="3" r="B28">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
         <v>210</v>
       </c>
-      <c t="s" s="3" r="D28">
+      <c r="D28" s="3" t="s">
         <v>211</v>
       </c>
-      <c t="s" s="3" r="E28">
+      <c r="E28" s="3" t="s">
         <v>212</v>
       </c>
-      <c t="s" s="3" r="F28">
+      <c r="F28" s="3" t="s">
         <v>213</v>
       </c>
-      <c t="s" s="3" r="G28">
+      <c r="G28" s="3" t="s">
         <v>214</v>
       </c>
-      <c t="s" s="3" r="H28">
+      <c r="H28" s="3" t="s">
         <v>215</v>
       </c>
-      <c t="s" s="3" r="I28">
+      <c r="I28" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="29">
-      <c t="s" s="3" r="B29">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
         <v>217</v>
       </c>
-      <c t="s" s="3" r="D29">
+      <c r="D29" s="3" t="s">
         <v>218</v>
       </c>
-      <c t="s" s="3" r="E29">
+      <c r="E29" s="3" t="s">
         <v>219</v>
       </c>
-      <c t="s" s="3" r="F29">
+      <c r="F29" s="3" t="s">
         <v>220</v>
       </c>
-      <c t="s" s="3" r="G29">
+      <c r="G29" s="3" t="s">
         <v>221</v>
       </c>
-      <c t="s" s="3" r="H29">
+      <c r="H29" s="3" t="s">
         <v>222</v>
       </c>
-      <c t="s" s="3" r="I29">
+      <c r="I29" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="30">
-      <c t="s" s="3" r="B30">
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
         <v>224</v>
       </c>
-      <c t="s" s="3" r="D30">
+      <c r="D30" s="3" t="s">
         <v>225</v>
       </c>
-      <c t="s" s="3" r="E30">
+      <c r="E30" s="3" t="s">
         <v>226</v>
       </c>
-      <c t="s" s="3" r="F30">
+      <c r="F30" s="3" t="s">
         <v>227</v>
       </c>
-      <c t="s" s="3" r="G30">
+      <c r="G30" s="3" t="s">
         <v>228</v>
       </c>
-      <c t="s" s="3" r="H30">
+      <c r="H30" s="3" t="s">
         <v>229</v>
       </c>
-      <c t="s" s="3" r="I30">
+      <c r="I30" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="31">
-      <c t="s" s="3" r="B31">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
         <v>231</v>
       </c>
-      <c t="s" s="3" r="D31">
+      <c r="D31" s="3" t="s">
         <v>232</v>
       </c>
-      <c t="s" s="3" r="E31">
+      <c r="E31" s="3" t="s">
         <v>233</v>
       </c>
-      <c t="s" s="3" r="F31">
+      <c r="F31" s="3" t="s">
         <v>234</v>
       </c>
-      <c t="s" s="3" r="G31">
+      <c r="G31" s="3" t="s">
         <v>235</v>
       </c>
-      <c t="s" s="3" r="H31">
+      <c r="H31" s="3" t="s">
         <v>236</v>
       </c>
-      <c t="s" s="3" r="I31">
+      <c r="I31" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="32">
-      <c t="s" s="3" r="B32">
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
         <v>238</v>
       </c>
-      <c t="s" s="3" r="D32">
+      <c r="D32" s="3" t="s">
         <v>239</v>
       </c>
-      <c t="s" s="3" r="E32">
+      <c r="E32" s="3" t="s">
         <v>240</v>
       </c>
-      <c t="s" s="3" r="F32">
+      <c r="F32" s="3" t="s">
         <v>241</v>
       </c>
-      <c t="s" s="3" r="G32">
+      <c r="G32" s="3" t="s">
         <v>242</v>
       </c>
-      <c t="s" s="3" r="H32">
+      <c r="H32" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="33">
-      <c t="s" s="3" r="B33">
+    <row r="33" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
         <v>244</v>
       </c>
-      <c t="s" s="3" r="D33">
+      <c r="D33" s="3" t="s">
         <v>245</v>
       </c>
-      <c t="s" s="3" r="E33">
+      <c r="E33" s="3" t="s">
         <v>246</v>
       </c>
-      <c t="s" s="3" r="G33">
+      <c r="G33" s="3" t="s">
         <v>247</v>
       </c>
-      <c t="s" s="3" r="H33">
+      <c r="H33" s="3" t="s">
         <v>248</v>
       </c>
-      <c t="s" s="3" r="I33">
+      <c r="I33" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="34">
-      <c t="s" s="3" r="B34">
+    <row r="34" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
         <v>250</v>
       </c>
-      <c t="s" s="3" r="D34">
+      <c r="D34" s="3" t="s">
         <v>251</v>
       </c>
-      <c t="s" s="3" r="E34">
+      <c r="E34" s="3" t="s">
         <v>252</v>
       </c>
-      <c t="s" s="3" r="F34">
+      <c r="F34" s="3" t="s">
         <v>253</v>
       </c>
-      <c t="s" s="3" r="G34">
+      <c r="G34" s="3" t="s">
         <v>254</v>
       </c>
-      <c t="s" s="3" r="H34">
+      <c r="H34" s="3" t="s">
         <v>255</v>
       </c>
-      <c t="s" s="3" r="I34">
+      <c r="I34" s="3" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="35">
-      <c t="s" s="3" r="B35">
+    <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
         <v>257</v>
       </c>
-      <c t="s" s="3" r="D35">
+      <c r="D35" s="3" t="s">
         <v>258</v>
       </c>
-      <c t="s" s="3" r="E35">
+      <c r="E35" s="3" t="s">
         <v>259</v>
       </c>
-      <c t="s" s="4" r="F35">
+      <c r="F35" s="4" t="s">
         <v>260</v>
       </c>
-      <c t="s" s="3" r="G35">
+      <c r="G35" s="3" t="s">
         <v>261</v>
       </c>
-      <c t="s" s="3" r="H35">
+      <c r="H35" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="36">
-      <c t="s" s="3" r="B36">
+    <row r="36" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
         <v>263</v>
       </c>
-      <c t="s" s="3" r="D36">
+      <c r="D36" s="3" t="s">
         <v>264</v>
       </c>
-      <c t="s" s="3" r="E36">
+      <c r="E36" s="3" t="s">
         <v>265</v>
       </c>
-      <c t="s" s="4" r="F36">
+      <c r="F36" s="4" t="s">
         <v>266</v>
       </c>
-      <c t="s" s="3" r="G36">
+      <c r="G36" s="3" t="s">
         <v>267</v>
       </c>
-      <c t="s" s="3" r="H36">
+      <c r="H36" s="3" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="37">
-      <c t="s" s="3" r="B37">
+      <c r="I36" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
         <v>269</v>
       </c>
-      <c t="s" s="3" r="D37">
+      <c r="D37" s="3" t="s">
         <v>270</v>
       </c>
-      <c t="s" s="3" r="E37">
+      <c r="E37" s="3" t="s">
         <v>271</v>
       </c>
-      <c t="s" s="4" r="F37">
+      <c r="F37" s="4" t="s">
         <v>272</v>
       </c>
-      <c t="s" s="3" r="G37">
+      <c r="G37" s="3" t="s">
         <v>273</v>
       </c>
-      <c t="s" s="3" r="H37">
+      <c r="H37" s="3" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="38">
-      <c t="s" s="3" r="B38">
+      <c r="I37" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
         <v>275</v>
       </c>
-      <c t="s" s="3" r="D38">
+      <c r="D38" s="3" t="s">
         <v>276</v>
       </c>
-      <c t="s" s="3" r="E38">
+      <c r="E38" s="3" t="s">
         <v>277</v>
       </c>
-      <c t="s" s="4" r="F38">
+      <c r="F38" s="4" t="s">
         <v>278</v>
       </c>
-      <c t="s" s="3" r="G38">
+      <c r="G38" s="3" t="s">
         <v>279</v>
       </c>
-      <c t="s" s="3" r="H38">
+      <c r="H38" s="3" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="39">
-      <c t="s" s="3" r="B39">
+      <c r="I38" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B39" s="3" t="s">
         <v>281</v>
       </c>
-      <c t="s" s="3" r="D39">
+      <c r="D39" s="3" t="s">
         <v>282</v>
       </c>
-      <c t="s" s="3" r="E39">
+      <c r="E39" s="3" t="s">
         <v>283</v>
       </c>
-      <c t="s" s="4" r="F39">
+      <c r="F39" s="4" t="s">
         <v>284</v>
       </c>
-      <c t="s" s="3" r="G39">
+      <c r="G39" s="3" t="s">
         <v>285</v>
       </c>
-      <c t="s" s="3" r="H39">
+      <c r="H39" s="3" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="40">
-      <c t="s" s="3" r="B40">
+      <c r="I39" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
         <v>287</v>
       </c>
-      <c t="s" s="3" r="D40">
+      <c r="D40" s="3" t="s">
         <v>288</v>
       </c>
-      <c t="s" s="3" r="E40">
+      <c r="E40" s="3" t="s">
         <v>289</v>
       </c>
-      <c t="s" s="4" r="F40">
+      <c r="F40" s="4" t="s">
         <v>290</v>
       </c>
-      <c t="s" s="3" r="G40">
+      <c r="G40" s="3" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="41">
-      <c t="s" s="3" r="B41">
+      <c r="I40" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
         <v>292</v>
       </c>
-      <c t="s" s="4" r="F41">
+      <c r="F41" s="4" t="s">
         <v>293</v>
       </c>
-      <c t="s" s="3" r="H41">
+      <c r="H41" s="3" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="42">
-      <c t="s" s="3" r="B42">
+      <c r="I41" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
         <v>295</v>
       </c>
-      <c t="s" s="3" r="D42">
+      <c r="D42" s="3" t="s">
         <v>296</v>
       </c>
-      <c t="s" s="3" r="E42">
+      <c r="E42" s="3" t="s">
         <v>297</v>
       </c>
-      <c t="s" s="4" r="F42">
+      <c r="F42" s="4" t="s">
         <v>298</v>
       </c>
-      <c t="s" s="3" r="G42">
+      <c r="G42" s="3" t="s">
         <v>299</v>
       </c>
-      <c t="s" s="3" r="H42">
+      <c r="H42" s="3" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="43">
-      <c t="s" s="3" r="B43">
+      <c r="I42" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
         <v>301</v>
       </c>
-      <c t="s" s="4" r="D43">
+      <c r="D43" s="4" t="s">
         <v>302</v>
       </c>
-      <c t="s" s="4" r="E43">
+      <c r="E43" s="4" t="s">
         <v>303</v>
       </c>
-      <c t="s" s="4" r="F43">
+      <c r="F43" s="4" t="s">
         <v>304</v>
       </c>
-      <c t="s" s="3" r="G43">
+      <c r="G43" s="3" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="44">
-      <c t="s" s="4" r="D44">
+      <c r="I43" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D44" s="4" t="s">
         <v>306</v>
       </c>
-      <c t="s" s="4" r="E44">
+      <c r="E44" s="4" t="s">
         <v>307</v>
       </c>
-      <c t="s" s="4" r="F44">
+      <c r="F44" s="4" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="45">
-      <c t="s" s="4" r="D45">
+      <c r="H44" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D45" s="4" t="s">
         <v>309</v>
       </c>
-      <c t="s" s="4" r="E45">
+      <c r="E45" s="4" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="46">
-      <c t="s" s="4" r="D46">
+      <c r="G45" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D46" s="4" t="s">
         <v>311</v>
       </c>
-      <c t="s" s="4" r="E46">
+      <c r="E46" s="4" t="s">
         <v>312</v>
       </c>
-      <c t="s" s="3" r="G46">
+      <c r="G46" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D47" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D48" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D49" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="D50" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D51" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D52" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G53" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G54" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G55" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G56" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G57" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G58" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G59" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G62" s="3" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="47">
-      <c t="s" s="4" r="D47">
-        <v>314</v>
-      </c>
-      <c t="s" s="4" r="E47">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="48">
-      <c t="s" s="4" r="D48">
-        <v>316</v>
-      </c>
-      <c t="s" s="4" r="E48">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="49">
-      <c t="s" s="4" r="D49">
-        <v>318</v>
-      </c>
-      <c t="s" s="4" r="E49">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="50">
-      <c s="3" r="A50"/>
-      <c t="s" s="4" r="D50">
-        <v>320</v>
-      </c>
-      <c t="s" s="4" r="E50">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="51">
-      <c t="s" s="4" r="D51">
-        <v>322</v>
-      </c>
-      <c t="s" s="4" r="E51">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="52">
-      <c t="s" s="4" r="D52">
-        <v>324</v>
-      </c>
-      <c t="s" s="4" r="E52">
-        <v>325</v>
-      </c>
-    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c t="s" s="3" r="A1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>326</v>
       </c>
-      <c t="s" s="3" r="B1">
+      <c r="B1" s="3" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="3" r="A2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>328</v>
       </c>
-      <c t="s" s="3" r="B2">
+      <c r="B2" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="3" r="A3">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>330</v>
       </c>
-      <c t="s" s="3" r="B3">
+      <c r="B3" s="3" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" s="3" r="A4">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>332</v>
       </c>
-      <c t="s" s="3" r="B4">
+      <c r="B4" s="3" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" s="3" r="A5">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>334</v>
       </c>
-      <c t="s" s="3" r="B5">
+      <c r="B5" s="3" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" s="3" r="A6">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>336</v>
       </c>
-      <c t="s" s="3" r="B6">
+      <c r="B6" s="3" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" s="3" r="A7">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>338</v>
       </c>
-      <c t="s" s="3" r="B7">
+      <c r="B7" s="3" t="s">
         <v>339</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated documentation on document property collection
</commit_message>
<xml_diff>
--- a/docs/ClamAV_Document_Properties.xlsx
+++ b/docs/ClamAV_Document_Properties.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="375">
   <si>
     <t>All Documents</t>
   </si>
@@ -1077,13 +1077,76 @@
   </si>
   <si>
     <t>OOXML_ERROR_OUTOFMEM</t>
+  </si>
+  <si>
+    <t>MSXML Word (2003)</t>
+  </si>
+  <si>
+    <t>MSXML Excel (2003)</t>
+  </si>
+  <si>
+    <t>WordDocument(object)</t>
+  </si>
+  <si>
+    <t>Workbook(object)</t>
+  </si>
+  <si>
+    <t>Attributes(array)</t>
+  </si>
+  <si>
+    <t>BinaryData(int)</t>
+  </si>
+  <si>
+    <t>DocumentProperties(object)</t>
+  </si>
+  <si>
+    <t>TotalTime(string)*</t>
+  </si>
+  <si>
+    <t>LastSaved(string)*</t>
+  </si>
+  <si>
+    <t>Paragraph(int)*</t>
+  </si>
+  <si>
+    <t>Version(int)*</t>
+  </si>
+  <si>
+    <t>AllowPNG(boolean)*</t>
+  </si>
+  <si>
+    <t>OOXML_ERROR_XML_READER_IO</t>
+  </si>
+  <si>
+    <t>MSXML_RECURSIVE_LIMIT</t>
+  </si>
+  <si>
+    <t>MSXML_NAMELESS_ELEMENT</t>
+  </si>
+  <si>
+    <t>MSXML_INTR_VIRUS</t>
+  </si>
+  <si>
+    <t>MSXML_INTR_TIMEOUT</t>
+  </si>
+  <si>
+    <t>MSXML_ERROR_XMLPARSER</t>
+  </si>
+  <si>
+    <t>MSXML_ERROR_OUTOFMEM</t>
+  </si>
+  <si>
+    <t>MSXML_ERROR_MALFORMED</t>
+  </si>
+  <si>
+    <t>MSXML_ERROR_OTHER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1109,6 +1172,17 @@
     </font>
     <font>
       <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1144,13 +1218,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1454,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E34" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1464,7 +1549,7 @@
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" customWidth="1"/>
     <col min="4" max="6" width="45.5703125" customWidth="1"/>
-    <col min="7" max="9" width="38" customWidth="1"/>
+    <col min="7" max="11" width="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1495,8 +1580,12 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="J1" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>355</v>
+      </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1541,6 +1630,12 @@
       <c r="I2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="J2" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -1570,6 +1665,12 @@
       <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="J3" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -1599,6 +1700,10 @@
       <c r="I4" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="J4" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -1628,6 +1733,10 @@
       <c r="I5" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -1648,6 +1757,12 @@
       <c r="I6" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="J6" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -1668,6 +1783,12 @@
       <c r="F7" s="3" t="s">
         <v>56</v>
       </c>
+      <c r="J7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
@@ -1694,6 +1815,12 @@
       <c r="I8" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="J8" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
@@ -1720,6 +1847,12 @@
       <c r="I9" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="J9" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
@@ -1746,6 +1879,12 @@
       <c r="I10" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="J10" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
@@ -1772,6 +1911,12 @@
       <c r="I11" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="J11" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
@@ -1798,6 +1943,12 @@
       <c r="I12" s="3" t="s">
         <v>96</v>
       </c>
+      <c r="J12" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
@@ -1824,6 +1975,12 @@
       <c r="I13" s="3" t="s">
         <v>104</v>
       </c>
+      <c r="J13" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
@@ -1850,6 +2007,12 @@
       <c r="I14" s="3" t="s">
         <v>112</v>
       </c>
+      <c r="J14" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
@@ -1876,6 +2039,12 @@
       <c r="I15" s="3" t="s">
         <v>120</v>
       </c>
+      <c r="J15" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
@@ -1902,8 +2071,14 @@
       <c r="I16" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J16" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>129</v>
       </c>
@@ -1928,8 +2103,14 @@
       <c r="I17" s="3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J17" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>137</v>
       </c>
@@ -1954,8 +2135,14 @@
       <c r="I18" s="3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J18" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>145</v>
       </c>
@@ -1980,8 +2167,14 @@
       <c r="I19" s="3" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J19" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>153</v>
       </c>
@@ -2003,8 +2196,12 @@
       <c r="H20" s="3" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J20" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>160</v>
       </c>
@@ -2020,8 +2217,12 @@
       <c r="I21" s="3" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J21" s="7"/>
+      <c r="K21" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>165</v>
       </c>
@@ -2043,8 +2244,14 @@
       <c r="I22" s="3" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J22" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>172</v>
       </c>
@@ -2069,8 +2276,14 @@
       <c r="I23" s="3" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J23" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>180</v>
       </c>
@@ -2095,8 +2308,14 @@
       <c r="I24" s="3" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J24" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>188</v>
       </c>
@@ -2121,8 +2340,14 @@
       <c r="I25" s="3" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J25" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>196</v>
       </c>
@@ -2141,8 +2366,14 @@
       <c r="I26" s="3" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J26" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>202</v>
       </c>
@@ -2167,8 +2398,14 @@
       <c r="I27" s="3" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J27" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
         <v>210</v>
       </c>
@@ -2190,8 +2427,14 @@
       <c r="I28" s="3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J28" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
         <v>217</v>
       </c>
@@ -2213,8 +2456,14 @@
       <c r="I29" s="3" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J29" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
         <v>224</v>
       </c>
@@ -2236,8 +2485,14 @@
       <c r="I30" s="3" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J30" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
         <v>231</v>
       </c>
@@ -2259,8 +2514,12 @@
       <c r="I31" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J31" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
         <v>238</v>
       </c>
@@ -2279,8 +2538,10 @@
       <c r="H32" s="3" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="33" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
         <v>244</v>
       </c>
@@ -2299,8 +2560,10 @@
       <c r="I33" s="3" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
         <v>250</v>
       </c>
@@ -2322,8 +2585,10 @@
       <c r="I34" s="3" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+    </row>
+    <row r="35" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
         <v>257</v>
       </c>
@@ -2343,7 +2608,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
         <v>263</v>
       </c>
@@ -2366,7 +2631,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
         <v>269</v>
       </c>
@@ -2389,7 +2654,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="38" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
         <v>275</v>
       </c>
@@ -2412,7 +2677,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="39" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>281</v>
       </c>
@@ -2435,7 +2700,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="40" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
         <v>287</v>
       </c>
@@ -2455,7 +2720,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="41" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
         <v>292</v>
       </c>
@@ -2469,7 +2734,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="42" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>295</v>
       </c>
@@ -2492,7 +2757,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="43" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>301</v>
       </c>
@@ -2512,7 +2777,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D44" s="4" t="s">
         <v>306</v>
       </c>
@@ -2529,7 +2794,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D45" s="4" t="s">
         <v>309</v>
       </c>
@@ -2546,7 +2811,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="46" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D46" s="4" t="s">
         <v>311</v>
       </c>
@@ -2563,7 +2828,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="47" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D47" s="4" t="s">
         <v>314</v>
       </c>
@@ -2580,7 +2845,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="48" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D48" s="4" t="s">
         <v>316</v>
       </c>

</xml_diff>